<commit_message>
Update default excel templates to current cidc-schemas version
</commit_message>
<xml_diff>
--- a/public/static/xlsx/metadata/cytof_template.xlsx
+++ b/public/static/xlsx/metadata/cytof_template.xlsx
@@ -7,9 +7,8 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Data Acquisition" sheetId="1" r:id="rId1"/>
-    <sheet name="Data Preprocessing" sheetId="2" r:id="rId2"/>
-    <sheet name="Antibody Information" sheetId="3" r:id="rId3"/>
+    <sheet name="Acquisition and Preprocessing" sheetId="1" r:id="rId1"/>
+    <sheet name="Antibody Information" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -30,7 +29,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Trial identifier used by lead organization, e.g. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
+          <t>Trial identifier used by lead organization, ie. Center for Experimental Therapeutics Program (CTEP) ID or Industry Sponsored ID.  This is usually a short identifier. Example: E4412.</t>
         </r>
       </text>
     </comment>
@@ -56,7 +55,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Assay category.</t>
+          <t>Standardized CyTOF panel name used for antibody sample development.</t>
         </r>
       </text>
     </comment>
@@ -69,11 +68,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Artifact category.</t>
+          <t>Name of CyTOF instrument on which experiment was conducted.</t>
         </r>
       </text>
     </comment>
-    <comment ref="B6" authorId="0">
+    <comment ref="B8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -82,11 +81,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Standardized CyTOF panel name used for antibody sample development.</t>
+          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Formated as CM-????-????-??</t>
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -95,11 +94,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Normalized cyTOF FCS filenames.</t>
+          <t>CyTOF batch identification number.</t>
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="D8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -108,11 +107,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Date of cyTOF batch acquisition.</t>
+          <t>Path to a file on a user's computer.</t>
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -121,11 +120,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>CyTOF instrument used for experiment.</t>
+          <t>Date of CyTOF batch acquisition.</t>
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="F8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -138,7 +137,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -151,7 +150,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="H8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -160,11 +159,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>CyTOF batch identifaction number.</t>
+          <t>Analysis rate of CyTOF expressions per second.</t>
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0">
+    <comment ref="I8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -173,11 +172,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Analysis rate of cyTOF expressions per second.</t>
+          <t>Length of run time for CyTOF experiment.</t>
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0">
+    <comment ref="J8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -186,99 +185,11 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Length of run time for cyTOF experiment.</t>
+          <t>Path to a file on a user's computer.</t>
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Any notes pertaining to cyTOF acquisition.</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
-<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <authors>
-    <author>CIDC</author>
-  </authors>
-  <commentList>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Participant identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-1234.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="C2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Specimen identifier assigned by the CIMAC-CIDC Network. Example: CIMAC-12453.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="D2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Study related collection time point, as described in the protocol intake form. Example: Progression.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="E2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a users computer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Path to a file on a users computer</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="K8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -291,7 +202,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H2" authorId="0">
+    <comment ref="L8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -304,7 +215,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I2" authorId="0">
+    <comment ref="M8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -317,7 +228,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J2" authorId="0">
+    <comment ref="N8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -330,7 +241,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K2" authorId="0">
+    <comment ref="O8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -343,7 +254,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L2" authorId="0">
+    <comment ref="P8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -352,7 +263,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Identification number for CyTOF assay batch.</t>
+          <t>Any notes pertaining to preprocessing of CyTOF data.</t>
         </r>
       </text>
     </comment>
@@ -360,7 +271,7 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>CIDC</author>
@@ -470,38 +381,51 @@
         </r>
       </text>
     </comment>
+    <comment ref="J2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>How this antibody should be used in automatic analysis</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="36">
   <si>
     <t>#t</t>
   </si>
   <si>
-    <t>METADATA FILE FOR CYTOF</t>
+    <t>Metadata file for cytof</t>
   </si>
   <si>
     <t>#p</t>
   </si>
   <si>
-    <t>LEAD ORGANIZATION STUDY ID</t>
-  </si>
-  <si>
-    <t>ASSAY CREATOR</t>
-  </si>
-  <si>
-    <t>ASSAY CATEGORY</t>
-  </si>
-  <si>
-    <t>ARTIFACT CATEGORY</t>
-  </si>
-  <si>
-    <t>PANEL NAME</t>
-  </si>
-  <si>
-    <t>Runs</t>
+    <t>Protocol identifier</t>
+  </si>
+  <si>
+    <t>Assay creator</t>
+  </si>
+  <si>
+    <t>Panel name</t>
+  </si>
+  <si>
+    <t>Instrument</t>
+  </si>
+  <si>
+    <t>Run info</t>
+  </si>
+  <si>
+    <t>Preprocessing</t>
   </si>
   <si>
     <t>#h</t>
@@ -510,91 +434,79 @@
     <t>#d</t>
   </si>
   <si>
-    <t>ORIGINAL FCS FILENAME(S)</t>
-  </si>
-  <si>
-    <t>DATE OF ACQUISITION</t>
-  </si>
-  <si>
-    <t>INSTRUMENT</t>
-  </si>
-  <si>
-    <t>INJECTOR</t>
-  </si>
-  <si>
-    <t>ACQUISITION_BUFFER</t>
-  </si>
-  <si>
-    <t>BATCH_ID</t>
-  </si>
-  <si>
-    <t>AVERAGE_EVENT_PER_SECOND</t>
-  </si>
-  <si>
-    <t>RUN_TIME</t>
-  </si>
-  <si>
-    <t>NOTES</t>
+    <t>Cimac id</t>
+  </si>
+  <si>
+    <t>Batch_id</t>
+  </si>
+  <si>
+    <t>Original fcs filename(s)</t>
+  </si>
+  <si>
+    <t>Date of acquisition</t>
+  </si>
+  <si>
+    <t>Injector</t>
+  </si>
+  <si>
+    <t>Acquisition_buffer</t>
+  </si>
+  <si>
+    <t>Average_event_per_second</t>
+  </si>
+  <si>
+    <t>Run_time</t>
+  </si>
+  <si>
+    <t>Processed fcs filename</t>
+  </si>
+  <si>
+    <t>Concatenation version</t>
+  </si>
+  <si>
+    <t>Normalization version</t>
+  </si>
+  <si>
+    <t>Beads removed</t>
+  </si>
+  <si>
+    <t>Debarcoding protocol</t>
+  </si>
+  <si>
+    <t>Debarcoding key</t>
+  </si>
+  <si>
+    <t>Preprocessing_notes</t>
   </si>
   <si>
     <t>Samples</t>
   </si>
   <si>
-    <t>CIMAC PARTICPANT ID</t>
-  </si>
-  <si>
-    <t>CIMAC SAMPLE ID</t>
-  </si>
-  <si>
-    <t>TIME POINT</t>
-  </si>
-  <si>
-    <t>PROCESSED FCS FILENAME</t>
-  </si>
-  <si>
-    <t>SOURCE FCS FILENAMES</t>
-  </si>
-  <si>
-    <t>CONCATENATION VERSION</t>
-  </si>
-  <si>
-    <t>NORMALIZATION VERSION</t>
-  </si>
-  <si>
-    <t>BEADS REMOVED</t>
-  </si>
-  <si>
-    <t>DEBARCODING PROTOCOL</t>
-  </si>
-  <si>
-    <t>DEBARCODING KEY</t>
-  </si>
-  <si>
-    <t>BATCH ID</t>
-  </si>
-  <si>
-    <t>TARGET</t>
-  </si>
-  <si>
-    <t>CLONE</t>
-  </si>
-  <si>
-    <t>ANTIBODY COMPANY</t>
-  </si>
-  <si>
-    <t>CATALOG NUMBER</t>
-  </si>
-  <si>
-    <t>LOT NUMBER</t>
-  </si>
-  <si>
-    <t>ISOTOPE</t>
-  </si>
-  <si>
-    <t>DILUTION</t>
-  </si>
-  <si>
-    <t>STAIN_TYPE</t>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Clone</t>
+  </si>
+  <si>
+    <t>Antibody company</t>
+  </si>
+  <si>
+    <t>Catalog number</t>
+  </si>
+  <si>
+    <t>Lot number</t>
+  </si>
+  <si>
+    <t>Isotope</t>
+  </si>
+  <si>
+    <t>Dilution</t>
+  </si>
+  <si>
+    <t>Stain_type</t>
+  </si>
+  <si>
+    <t>Usage</t>
   </si>
 </sst>
 </file>
@@ -994,7 +906,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J209"/>
+  <dimension ref="A1:P208"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1004,1183 +916,12 @@
     <col min="2" max="101" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:16">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10">
-      <c r="A12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10">
-      <c r="A15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1">
-      <c r="A18" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1">
-      <c r="A19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1">
-      <c r="A20" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1">
-      <c r="A23" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1">
-      <c r="A24" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1">
-      <c r="A25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1">
-      <c r="A26" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1">
-      <c r="A27" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1">
-      <c r="A28" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1">
-      <c r="A30" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1">
-      <c r="A31" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1">
-      <c r="A32" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1">
-      <c r="A33" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1">
-      <c r="A34" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1">
-      <c r="A35" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1">
-      <c r="A36" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1">
-      <c r="A37" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1">
-      <c r="A39" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1">
-      <c r="A41" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1">
-      <c r="A43" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1">
-      <c r="A44" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1">
-      <c r="A45" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1">
-      <c r="A46" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1">
-      <c r="A47" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1">
-      <c r="A49" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1">
-      <c r="A50" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="51" spans="1:1">
-      <c r="A51" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:1">
-      <c r="A52" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="53" spans="1:1">
-      <c r="A53" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="54" spans="1:1">
-      <c r="A54" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="55" spans="1:1">
-      <c r="A55" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:1">
-      <c r="A56" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="57" spans="1:1">
-      <c r="A57" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="58" spans="1:1">
-      <c r="A58" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="59" spans="1:1">
-      <c r="A59" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="60" spans="1:1">
-      <c r="A60" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="61" spans="1:1">
-      <c r="A61" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="62" spans="1:1">
-      <c r="A62" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="63" spans="1:1">
-      <c r="A63" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="64" spans="1:1">
-      <c r="A64" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="65" spans="1:1">
-      <c r="A65" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="66" spans="1:1">
-      <c r="A66" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="67" spans="1:1">
-      <c r="A67" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="68" spans="1:1">
-      <c r="A68" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="69" spans="1:1">
-      <c r="A69" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="70" spans="1:1">
-      <c r="A70" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="71" spans="1:1">
-      <c r="A71" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="72" spans="1:1">
-      <c r="A72" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="73" spans="1:1">
-      <c r="A73" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="74" spans="1:1">
-      <c r="A74" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1">
-      <c r="A75" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="76" spans="1:1">
-      <c r="A76" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1">
-      <c r="A77" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="78" spans="1:1">
-      <c r="A78" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="79" spans="1:1">
-      <c r="A79" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="80" spans="1:1">
-      <c r="A80" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1">
-      <c r="A81" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="82" spans="1:1">
-      <c r="A82" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="83" spans="1:1">
-      <c r="A83" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="84" spans="1:1">
-      <c r="A84" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="85" spans="1:1">
-      <c r="A85" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="86" spans="1:1">
-      <c r="A86" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="87" spans="1:1">
-      <c r="A87" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="88" spans="1:1">
-      <c r="A88" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="89" spans="1:1">
-      <c r="A89" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="90" spans="1:1">
-      <c r="A90" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="91" spans="1:1">
-      <c r="A91" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="92" spans="1:1">
-      <c r="A92" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="93" spans="1:1">
-      <c r="A93" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="94" spans="1:1">
-      <c r="A94" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="95" spans="1:1">
-      <c r="A95" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="96" spans="1:1">
-      <c r="A96" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="97" spans="1:1">
-      <c r="A97" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="98" spans="1:1">
-      <c r="A98" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="99" spans="1:1">
-      <c r="A99" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="100" spans="1:1">
-      <c r="A100" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="101" spans="1:1">
-      <c r="A101" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="102" spans="1:1">
-      <c r="A102" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="103" spans="1:1">
-      <c r="A103" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="104" spans="1:1">
-      <c r="A104" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="105" spans="1:1">
-      <c r="A105" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="106" spans="1:1">
-      <c r="A106" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="107" spans="1:1">
-      <c r="A107" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="108" spans="1:1">
-      <c r="A108" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="109" spans="1:1">
-      <c r="A109" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="110" spans="1:1">
-      <c r="A110" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="111" spans="1:1">
-      <c r="A111" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="112" spans="1:1">
-      <c r="A112" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="113" spans="1:1">
-      <c r="A113" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1">
-      <c r="A114" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1">
-      <c r="A115" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1">
-      <c r="A116" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1">
-      <c r="A117" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1">
-      <c r="A118" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1">
-      <c r="A119" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1">
-      <c r="A120" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1">
-      <c r="A121" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1">
-      <c r="A122" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1">
-      <c r="A123" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1">
-      <c r="A124" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1">
-      <c r="A125" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1">
-      <c r="A126" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1">
-      <c r="A127" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1">
-      <c r="A128" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1">
-      <c r="A129" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1">
-      <c r="A130" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1">
-      <c r="A131" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1">
-      <c r="A132" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1">
-      <c r="A133" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1">
-      <c r="A134" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1">
-      <c r="A135" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1">
-      <c r="A136" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1">
-      <c r="A137" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1">
-      <c r="A138" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1">
-      <c r="A139" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1">
-      <c r="A140" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1">
-      <c r="A141" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1">
-      <c r="A142" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1">
-      <c r="A143" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1">
-      <c r="A144" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1">
-      <c r="A145" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1">
-      <c r="A146" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1">
-      <c r="A147" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1">
-      <c r="A148" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1">
-      <c r="A149" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1">
-      <c r="A150" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1">
-      <c r="A151" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1">
-      <c r="A152" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1">
-      <c r="A153" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1">
-      <c r="A154" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1">
-      <c r="A155" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1">
-      <c r="A156" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1">
-      <c r="A157" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1">
-      <c r="A158" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="159" spans="1:1">
-      <c r="A159" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="160" spans="1:1">
-      <c r="A160" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="161" spans="1:1">
-      <c r="A161" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="162" spans="1:1">
-      <c r="A162" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="163" spans="1:1">
-      <c r="A163" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="164" spans="1:1">
-      <c r="A164" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="165" spans="1:1">
-      <c r="A165" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="166" spans="1:1">
-      <c r="A166" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="167" spans="1:1">
-      <c r="A167" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="168" spans="1:1">
-      <c r="A168" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="169" spans="1:1">
-      <c r="A169" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="170" spans="1:1">
-      <c r="A170" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="171" spans="1:1">
-      <c r="A171" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="172" spans="1:1">
-      <c r="A172" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="173" spans="1:1">
-      <c r="A173" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="174" spans="1:1">
-      <c r="A174" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="175" spans="1:1">
-      <c r="A175" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="176" spans="1:1">
-      <c r="A176" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="177" spans="1:1">
-      <c r="A177" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="178" spans="1:1">
-      <c r="A178" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="179" spans="1:1">
-      <c r="A179" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="180" spans="1:1">
-      <c r="A180" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="181" spans="1:1">
-      <c r="A181" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="182" spans="1:1">
-      <c r="A182" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="183" spans="1:1">
-      <c r="A183" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="184" spans="1:1">
-      <c r="A184" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="185" spans="1:1">
-      <c r="A185" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="186" spans="1:1">
-      <c r="A186" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="187" spans="1:1">
-      <c r="A187" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="188" spans="1:1">
-      <c r="A188" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="189" spans="1:1">
-      <c r="A189" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="190" spans="1:1">
-      <c r="A190" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="191" spans="1:1">
-      <c r="A191" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="192" spans="1:1">
-      <c r="A192" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="193" spans="1:1">
-      <c r="A193" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="194" spans="1:1">
-      <c r="A194" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="195" spans="1:1">
-      <c r="A195" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="196" spans="1:1">
-      <c r="A196" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="197" spans="1:1">
-      <c r="A197" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="198" spans="1:1">
-      <c r="A198" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="199" spans="1:1">
-      <c r="A199" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="200" spans="1:1">
-      <c r="A200" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="201" spans="1:1">
-      <c r="A201" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="202" spans="1:1">
-      <c r="A202" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="203" spans="1:1">
-      <c r="A203" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="204" spans="1:1">
-      <c r="A204" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="205" spans="1:1">
-      <c r="A205" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="206" spans="1:1">
-      <c r="A206" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="207" spans="1:1">
-      <c r="A207" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="208" spans="1:1">
-      <c r="A208" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="209" spans="1:1">
-      <c r="A209" t="s">
-        <v>10</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B1:J1"/>
-    <mergeCell ref="B8:J8"/>
-  </mergeCells>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
-      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C4">
-      <formula1>"Whole Exome Sequencing (WES),RNASeq,Conventional Immunohistochemistry,Multiplex Immunohistochemistry,Multiplex Immunofluorescence,CyTOF,OLink,NanoString,ELISpot,Multiplexed Ion-Beam Imaging (MIBI),Other,None"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C5">
-      <formula1>"Assay Artifact from CIMAC,Pipeline Artifact,Manifest File,Other"</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L202"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="2" max="101" width="30.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12">
-      <c r="B1" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -2192,111 +933,206 @@
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
-    </row>
-    <row r="2" spans="1:12">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" s="2"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="M8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="N8" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="O8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="P8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L2" s="4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12">
-      <c r="A7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12">
+    </row>
+    <row r="9" spans="1:16">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:16">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:16">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:16">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:16">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:16">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:16">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:16">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -3231,12 +2067,47 @@
         <v>10</v>
       </c>
     </row>
+    <row r="203" spans="1:1">
+      <c r="A203" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204" spans="1:1">
+      <c r="A204" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="205" spans="1:1">
+      <c r="A205" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="206" spans="1:1">
+      <c r="A206" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="207" spans="1:1">
+      <c r="A207" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="208" spans="1:1">
+      <c r="A208" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:L1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:P1"/>
+    <mergeCell ref="B7:I7"/>
+    <mergeCell ref="J7:P7"/>
   </mergeCells>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3">
+      <formula1>"DFCI,Mount Sinai,Stanford,MD Anderson"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M9:M208">
       <formula1>"Y,N"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3245,9 +2116,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I202"/>
+  <dimension ref="A1:J202"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3257,9 +2128,9 @@
     <col min="2" max="101" width="30.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:10">
       <c r="B1" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -3268,102 +2139,106 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" s="2"/>
+    </row>
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="H2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="I2" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="J2" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+    </row>
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:10">
       <c r="A5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:10">
       <c r="A6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:10">
       <c r="A7" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:10">
       <c r="A8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:10">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:10">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:10">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:10">
       <c r="A12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10">
       <c r="A13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:10">
       <c r="A14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:10">
       <c r="A15" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:10">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -4300,11 +3175,14 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="B1:I1"/>
+    <mergeCell ref="B1:J1"/>
   </mergeCells>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I202">
       <formula1>"Surface Stain,Intracellular"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J3:J202">
+      <formula1>"Ignored,Used,Analysis Only"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>